<commit_message>
added v1 of income statement dashboard for finance reports
</commit_message>
<xml_diff>
--- a/DataEngineering/finance_reports/income_statement_dashboard_data.xlsx
+++ b/DataEngineering/finance_reports/income_statement_dashboard_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17715"/>
   </bookViews>
   <sheets>
     <sheet name="actuals" sheetId="1" r:id="rId1"/>
@@ -93,8 +93,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="yyyy"/>
-    <numFmt numFmtId="169" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="yyyy"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -165,10 +165,10 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -178,13 +178,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -490,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,13 +531,13 @@
       </c>
       <c r="B2" s="7">
         <f>AVERAGE(C2:F2)</f>
-        <v>3367719.125</v>
+        <v>3517719.125</v>
       </c>
       <c r="C2" s="2">
-        <v>3537368.5</v>
+        <v>3937368.5</v>
       </c>
       <c r="D2" s="2">
-        <v>3323797.5</v>
+        <v>3523797.5</v>
       </c>
       <c r="E2" s="2">
         <v>3257922.5</v>
@@ -594,15 +594,15 @@
       </c>
       <c r="B5" s="6">
         <f>AVERAGE(C5:F5)</f>
-        <v>3962022.5</v>
+        <v>4112022.5</v>
       </c>
       <c r="C5" s="6">
         <f>SUM(C2:C4)</f>
-        <v>4161610</v>
+        <v>4561610</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:F5" si="0">SUM(D2:D4)</f>
-        <v>3910350</v>
+        <v>4110350</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="0"/>
@@ -625,20 +625,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <f>AVERAGE(C7:F7)</f>
-        <v>1629365.625</v>
+        <f t="shared" ref="B7:B13" si="1">AVERAGE(C7:F7)</f>
+        <v>1477365.625</v>
       </c>
       <c r="C7" s="2">
-        <v>1657200</v>
+        <v>1600200</v>
       </c>
       <c r="D7" s="2">
-        <v>1577640</v>
+        <v>1500640</v>
       </c>
       <c r="E7" s="2">
-        <v>1606027.5</v>
+        <v>1420027.5</v>
       </c>
       <c r="F7" s="2">
-        <v>1676595</v>
+        <v>1388595</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -650,8 +650,8 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <f>AVERAGE(C8:F8)</f>
-        <v>325873.125</v>
+        <f t="shared" si="1"/>
+        <v>318373.125</v>
       </c>
       <c r="C8" s="2">
         <v>331440</v>
@@ -663,7 +663,7 @@
         <v>321205.5</v>
       </c>
       <c r="F8" s="2">
-        <v>335319</v>
+        <v>305319</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -675,8 +675,8 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <f>AVERAGE(C9:F9)</f>
-        <v>217248.75</v>
+        <f t="shared" si="1"/>
+        <v>211748.75</v>
       </c>
       <c r="C9" s="2">
         <v>220960</v>
@@ -688,7 +688,7 @@
         <v>214137</v>
       </c>
       <c r="F9" s="2">
-        <v>223546</v>
+        <v>201546</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -700,127 +700,110 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <f>AVERAGE(C10:F10)</f>
-        <v>2172487.5</v>
+        <f t="shared" si="1"/>
+        <v>2007487.5</v>
       </c>
       <c r="C10" s="6">
         <f>SUM(C7:C9)</f>
-        <v>2209600</v>
+        <v>2152600</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10:F10" si="1">SUM(D7:D9)</f>
-        <v>2103520</v>
+        <f>SUM(D7:D9)</f>
+        <v>2026520</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="1"/>
-        <v>2141370</v>
+        <f>SUM(E7:E9)</f>
+        <v>1955370</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="1"/>
-        <v>2235460</v>
+        <f>SUM(F7:F9)</f>
+        <v>1895460</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="6">
-        <f>AVERAGE(C11:F11)</f>
-        <v>1789535</v>
-      </c>
-      <c r="C11" s="7">
-        <f>C5-C10</f>
-        <v>1952010</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" ref="D11:F11" si="2">D5-D10</f>
-        <v>1806830</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="2"/>
-        <v>1691480</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="2"/>
-        <v>1707820</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="1"/>
+        <v>2104535</v>
+      </c>
+      <c r="C12" s="7">
+        <f>C5-C10</f>
+        <v>2409010</v>
+      </c>
+      <c r="D12" s="7">
+        <f>D5-D10</f>
+        <v>2083830</v>
+      </c>
+      <c r="E12" s="7">
+        <f>E5-E10</f>
+        <v>1877480</v>
+      </c>
+      <c r="F12" s="7">
+        <f>F5-F10</f>
+        <v>2047820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8">
-        <f>AVERAGE(C12:F12)</f>
-        <v>0.45138068515240509</v>
-      </c>
-      <c r="C12" s="8">
-        <f>C11/C5</f>
-        <v>0.46905164107160452</v>
-      </c>
-      <c r="D12" s="8">
-        <f t="shared" ref="D12:F12" si="3">D11/D5</f>
-        <v>0.46206349815233932</v>
-      </c>
-      <c r="E12" s="8">
-        <f t="shared" si="3"/>
-        <v>0.44131129577207562</v>
-      </c>
-      <c r="F12" s="8">
-        <f t="shared" si="3"/>
-        <v>0.43309630561360085</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.5110586826244059</v>
+      </c>
+      <c r="C13" s="8">
+        <f>C12/C5</f>
+        <v>0.52810520846806286</v>
+      </c>
+      <c r="D13" s="8">
+        <f>D12/D5</f>
+        <v>0.50697142579099108</v>
+      </c>
+      <c r="E13" s="8">
+        <f>E12/E5</f>
+        <v>0.48983915363241454</v>
+      </c>
+      <c r="F13" s="8">
+        <f>F12/F5</f>
+        <v>0.5193189426061553</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="7">
-        <f>AVERAGE(C14:F14)</f>
-        <v>338715</v>
-      </c>
-      <c r="C14" s="2">
-        <v>372906</v>
-      </c>
-      <c r="D14" s="2">
-        <v>344802</v>
-      </c>
-      <c r="E14" s="2">
-        <v>329082</v>
-      </c>
-      <c r="F14" s="2">
-        <v>308070</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="A14" s="5"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="7">
         <f>AVERAGE(C15:F15)</f>
-        <v>141131.25</v>
+        <v>338715</v>
       </c>
       <c r="C15" s="2">
-        <v>155377.5</v>
+        <v>372906</v>
       </c>
       <c r="D15" s="2">
-        <v>143667.5</v>
+        <v>344802</v>
       </c>
       <c r="E15" s="2">
-        <v>137117.5</v>
+        <v>329082</v>
       </c>
       <c r="F15" s="2">
-        <v>128362.5</v>
+        <v>308070</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -829,23 +812,23 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="7">
         <f>AVERAGE(C16:F16)</f>
-        <v>84678.75</v>
+        <v>141131.25</v>
       </c>
       <c r="C16" s="2">
-        <v>93226.5</v>
+        <v>155377.5</v>
       </c>
       <c r="D16" s="2">
-        <v>86200.5</v>
+        <v>143667.5</v>
       </c>
       <c r="E16" s="2">
-        <v>82270.5</v>
+        <v>137117.5</v>
       </c>
       <c r="F16" s="2">
-        <v>77017.5</v>
+        <v>128362.5</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -853,24 +836,24 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>12</v>
+      <c r="A17" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B17" s="7">
         <f>AVERAGE(C17:F17)</f>
-        <v>564525</v>
-      </c>
-      <c r="C17" s="6">
-        <v>621510</v>
-      </c>
-      <c r="D17" s="6">
-        <v>574670</v>
-      </c>
-      <c r="E17" s="6">
-        <v>548470</v>
-      </c>
-      <c r="F17" s="6">
-        <v>513450</v>
+        <v>84678.75</v>
+      </c>
+      <c r="C17" s="2">
+        <v>93226.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>86200.5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>82270.5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>77017.5</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -879,80 +862,80 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7">
+        <f>AVERAGE(C18:F18)</f>
+        <v>564525</v>
+      </c>
+      <c r="C18" s="6">
+        <v>621510</v>
+      </c>
+      <c r="D18" s="6">
+        <v>574670</v>
+      </c>
+      <c r="E18" s="6">
+        <v>548470</v>
+      </c>
+      <c r="F18" s="6">
+        <v>513450</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6">
-        <f>AVERAGE(C18:F18)</f>
-        <v>1225010</v>
-      </c>
-      <c r="C18" s="6">
-        <f>C11-C17</f>
-        <v>1330500</v>
-      </c>
-      <c r="D18" s="6">
-        <f t="shared" ref="D18:F18" si="4">D11-D17</f>
-        <v>1232160</v>
-      </c>
-      <c r="E18" s="6">
-        <f t="shared" si="4"/>
-        <v>1143010</v>
-      </c>
-      <c r="F18" s="6">
-        <f t="shared" si="4"/>
-        <v>1194370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="B19" s="6">
+        <f>AVERAGE(C19:F19)</f>
+        <v>1540010</v>
+      </c>
+      <c r="C19" s="6">
+        <f>C12-C18</f>
+        <v>1787500</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" ref="D19:F19" si="2">D12-D18</f>
+        <v>1509160</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="2"/>
+        <v>1329010</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="2"/>
+        <v>1534370</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="7">
-        <f>AVERAGE(C20:F20)</f>
-        <v>14890</v>
-      </c>
-      <c r="C20" s="2">
-        <v>12840</v>
-      </c>
-      <c r="D20" s="2">
-        <v>10760</v>
-      </c>
-      <c r="E20" s="2">
-        <v>22600</v>
-      </c>
-      <c r="F20" s="2">
-        <v>13360</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="A20" s="4"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="7">
         <f>AVERAGE(C21:F21)</f>
-        <v>11167.5</v>
+        <v>14890</v>
       </c>
       <c r="C21" s="2">
-        <v>9630</v>
+        <v>12840</v>
       </c>
       <c r="D21" s="2">
-        <v>8070</v>
+        <v>10760</v>
       </c>
       <c r="E21" s="2">
-        <v>16950</v>
+        <v>22600</v>
       </c>
       <c r="F21" s="2">
-        <v>10020</v>
+        <v>13360</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -961,7 +944,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B22" s="7">
         <f>AVERAGE(C22:F22)</f>
@@ -985,53 +968,78 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7">
+        <f>AVERAGE(C23:F23)</f>
+        <v>11167.5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>9630</v>
+      </c>
+      <c r="D23" s="2">
+        <v>8070</v>
+      </c>
+      <c r="E23" s="2">
+        <v>16950</v>
+      </c>
+      <c r="F23" s="2">
+        <v>10020</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="6">
-        <f>AVERAGE(C23:F23)</f>
+      <c r="B24" s="6">
+        <f>AVERAGE(C24:F24)</f>
         <v>-7445</v>
       </c>
-      <c r="C23" s="6">
-        <f>C20-(C21+C22)</f>
+      <c r="C24" s="6">
+        <f>C21-(C22+C23)</f>
         <v>-6420</v>
       </c>
-      <c r="D23" s="6">
-        <f t="shared" ref="D23:F23" si="5">D20-(D21+D22)</f>
+      <c r="D24" s="6">
+        <f t="shared" ref="D24:F24" si="3">D21-(D22+D23)</f>
         <v>-5380</v>
       </c>
-      <c r="E23" s="6">
-        <f t="shared" si="5"/>
+      <c r="E24" s="6">
+        <f t="shared" si="3"/>
         <v>-11300</v>
       </c>
-      <c r="F23" s="6">
-        <f t="shared" si="5"/>
+      <c r="F24" s="6">
+        <f t="shared" si="3"/>
         <v>-6680</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="6">
-        <f>AVERAGE(C25:F25)</f>
-        <v>1232455</v>
-      </c>
-      <c r="C25" s="6">
-        <f>C18-C23</f>
-        <v>1336920</v>
-      </c>
-      <c r="D25" s="6">
-        <f t="shared" ref="D25:F25" si="6">D18-D23</f>
-        <v>1237540</v>
-      </c>
-      <c r="E25" s="6">
-        <f t="shared" si="6"/>
-        <v>1154310</v>
-      </c>
-      <c r="F25" s="6">
-        <f t="shared" si="6"/>
-        <v>1201050</v>
+      <c r="B26" s="6">
+        <f>AVERAGE(C26:F26)</f>
+        <v>1547455</v>
+      </c>
+      <c r="C26" s="6">
+        <f>C19-C24</f>
+        <v>1793920</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" ref="D26:F26" si="4">D19-D24</f>
+        <v>1514540</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="4"/>
+        <v>1340310</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="4"/>
+        <v>1541050</v>
       </c>
     </row>
   </sheetData>
@@ -1047,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1085,15 +1093,15 @@
         <v>2900000</v>
       </c>
       <c r="D2" s="2">
-        <f>C2*0.95</f>
+        <f t="shared" ref="D2:F4" si="0">C2*0.95</f>
         <v>2755000</v>
       </c>
       <c r="E2" s="2">
-        <f>D2*0.95</f>
+        <f t="shared" si="0"/>
         <v>2617250</v>
       </c>
       <c r="F2" s="2">
-        <f>E2*0.95</f>
+        <f t="shared" si="0"/>
         <v>2486387.5</v>
       </c>
     </row>
@@ -1102,22 +1110,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <f t="shared" ref="B3:B5" si="0">AVERAGE(C3:F3)</f>
+        <f t="shared" ref="B3:B5" si="1">AVERAGE(C3:F3)</f>
         <v>278240.625</v>
       </c>
       <c r="C3" s="2">
         <v>300000</v>
       </c>
       <c r="D3" s="2">
-        <f>C3*0.95</f>
+        <f t="shared" si="0"/>
         <v>285000</v>
       </c>
       <c r="E3" s="2">
-        <f>D3*0.95</f>
+        <f t="shared" si="0"/>
         <v>270750</v>
       </c>
       <c r="F3" s="2">
-        <f>E3*0.95</f>
+        <f t="shared" si="0"/>
         <v>257212.5</v>
       </c>
     </row>
@@ -1126,22 +1134,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46373.4375</v>
       </c>
       <c r="C4" s="2">
         <v>50000</v>
       </c>
       <c r="D4" s="2">
-        <f>C4*0.95</f>
+        <f t="shared" si="0"/>
         <v>47500</v>
       </c>
       <c r="E4" s="2">
-        <f>D4*0.95</f>
+        <f t="shared" si="0"/>
         <v>45125</v>
       </c>
       <c r="F4" s="2">
-        <f>E4*0.95</f>
+        <f t="shared" si="0"/>
         <v>42868.75</v>
       </c>
     </row>
@@ -1150,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3014273.4375</v>
       </c>
       <c r="C5" s="2">

</xml_diff>